<commit_message>
Double checking data transferred properly from original output into PnR summary.
</commit_message>
<xml_diff>
--- a/Data/PnR/Jan_Polyp_PnR.xlsx
+++ b/Data/PnR/Jan_Polyp_PnR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jennica Moffat\Documents\CSUNthesis\Data\PnR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3F7002-9F6E-4A45-9254-1639E4F0F0C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C4049E-E701-4A0B-BB7C-84C570822A94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9DE3BF4D-FA46-474F-BFB9-F399C340B799}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$217</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$217</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>PolypID</t>
   </si>
@@ -180,13 +180,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF1E1E1E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,10 +215,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,15 +534,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265D603E-FBC4-405A-8933-8CCF9B7CF3A0}">
-  <dimension ref="A1:I217"/>
+  <dimension ref="A1:J217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -564,7 +571,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -592,8 +599,12 @@
       <c r="I2">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2" s="3" t="str">
+        <f>IF(E2=C2,"Yes", "No")</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>15</v>
       </c>
@@ -621,8 +632,12 @@
       <c r="I3">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3" s="3" t="str">
+        <f t="shared" ref="J3:J66" si="0">IF(E3=C3,"Yes", "No")</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -650,8 +665,12 @@
       <c r="I4">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>16</v>
       </c>
@@ -679,8 +698,12 @@
       <c r="I5">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -708,8 +731,12 @@
       <c r="I6">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>18</v>
       </c>
@@ -737,8 +764,12 @@
       <c r="I7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -766,8 +797,12 @@
       <c r="I8">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>20</v>
       </c>
@@ -795,28 +830,32 @@
       <c r="I9">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>43851</v>
       </c>
-      <c r="C10">
-        <v>9.0399999999999994E-2</v>
-      </c>
-      <c r="D10">
-        <v>0.29370000000000002</v>
-      </c>
-      <c r="E10">
-        <v>-3.3333333333329662E-5</v>
-      </c>
-      <c r="F10">
-        <v>-2.5991666666666635E-2</v>
-      </c>
-      <c r="G10">
-        <v>-2.5958333333333306E-2</v>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
       </c>
       <c r="H10" t="s">
         <v>12</v>
@@ -824,8 +863,12 @@
       <c r="I10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>22</v>
       </c>
@@ -853,8 +896,12 @@
       <c r="I11">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -882,8 +929,12 @@
       <c r="I12">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>24</v>
       </c>
@@ -911,8 +962,12 @@
       <c r="I13">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>27</v>
       </c>
@@ -926,13 +981,13 @@
         <v>0.58140000000000003</v>
       </c>
       <c r="E14">
-        <v>-1.0405</v>
+        <v>-1.2189000000000001</v>
       </c>
       <c r="F14">
-        <v>0.58140000000000003</v>
+        <v>0.17285000000000006</v>
       </c>
       <c r="G14">
-        <v>1.6219000000000001</v>
+        <v>1.39175</v>
       </c>
       <c r="H14">
         <v>95</v>
@@ -940,8 +995,12 @@
       <c r="I14">
         <v>111</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>52</v>
       </c>
@@ -955,13 +1014,13 @@
         <v>0.34470000000000001</v>
       </c>
       <c r="E15">
-        <v>3.5099999999999999E-2</v>
+        <v>-0.14330000000000001</v>
       </c>
       <c r="F15">
-        <v>0.34470000000000001</v>
+        <v>-6.3849999999999962E-2</v>
       </c>
       <c r="G15">
-        <v>0.30959999999999999</v>
+        <v>7.9450000000000048E-2</v>
       </c>
       <c r="H15">
         <v>46</v>
@@ -969,8 +1028,12 @@
       <c r="I15">
         <v>73</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>28</v>
       </c>
@@ -984,13 +1047,13 @@
         <v>0.35770000000000002</v>
       </c>
       <c r="E16">
-        <v>0.11990000000000001</v>
+        <v>-5.8499999999999996E-2</v>
       </c>
       <c r="F16">
-        <v>0.35770000000000002</v>
+        <v>-5.0849999999999951E-2</v>
       </c>
       <c r="G16">
-        <v>0.23780000000000001</v>
+        <v>7.6500000000000457E-3</v>
       </c>
       <c r="H16">
         <v>12</v>
@@ -998,28 +1061,32 @@
       <c r="I16">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>53</v>
       </c>
       <c r="B17" s="1">
         <v>43850</v>
       </c>
-      <c r="C17">
-        <v>0.4269</v>
-      </c>
-      <c r="D17">
-        <v>0.57750000000000001</v>
-      </c>
-      <c r="E17">
-        <v>0.4269</v>
-      </c>
-      <c r="F17">
-        <v>0.57750000000000001</v>
-      </c>
-      <c r="G17">
-        <v>0.15060000000000001</v>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>12</v>
       </c>
       <c r="H17" t="s">
         <v>12</v>
@@ -1027,8 +1094,12 @@
       <c r="I17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>29</v>
       </c>
@@ -1042,13 +1113,13 @@
         <v>6.9800000000000001E-2</v>
       </c>
       <c r="E18">
-        <v>-0.4385</v>
+        <v>-0.6169</v>
       </c>
       <c r="F18">
-        <v>6.9800000000000001E-2</v>
+        <v>-0.33875</v>
       </c>
       <c r="G18">
-        <v>0.50829999999999997</v>
+        <v>0.27815000000000001</v>
       </c>
       <c r="H18">
         <v>58</v>
@@ -1056,8 +1127,12 @@
       <c r="I18">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>54</v>
       </c>
@@ -1071,13 +1146,13 @@
         <v>0.40839999999999999</v>
       </c>
       <c r="E19">
-        <v>0.17460000000000001</v>
+        <v>-3.7999999999999978E-3</v>
       </c>
       <c r="F19">
-        <v>0.40839999999999999</v>
+        <v>-1.4999999999998348E-4</v>
       </c>
       <c r="G19">
-        <v>0.23379999999999998</v>
+        <v>3.6500000000000143E-3</v>
       </c>
       <c r="H19">
         <v>103</v>
@@ -1085,8 +1160,12 @@
       <c r="I19">
         <v>110</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>32</v>
       </c>
@@ -1100,13 +1179,13 @@
         <v>0.36359999999999998</v>
       </c>
       <c r="E20">
-        <v>0.17680000000000001</v>
+        <v>-1.5999999999999903E-3</v>
       </c>
       <c r="F20">
-        <v>0.36359999999999998</v>
+        <v>-4.494999999999999E-2</v>
       </c>
       <c r="G20">
-        <v>0.18679999999999997</v>
+        <v>-4.335E-2</v>
       </c>
       <c r="H20">
         <v>70</v>
@@ -1114,8 +1193,12 @@
       <c r="I20">
         <v>91</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>56</v>
       </c>
@@ -1129,13 +1212,13 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="E21">
-        <v>6.2700000000000006E-2</v>
+        <v>-0.1157</v>
       </c>
       <c r="F21">
-        <v>0.28999999999999998</v>
+        <v>-0.11854999999999999</v>
       </c>
       <c r="G21">
-        <v>0.22729999999999997</v>
+        <v>-2.8499999999999914E-3</v>
       </c>
       <c r="H21">
         <v>63</v>
@@ -1143,8 +1226,12 @@
       <c r="I21">
         <v>54</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>33</v>
       </c>
@@ -1158,13 +1245,13 @@
         <v>1.1963999999999999</v>
       </c>
       <c r="E22">
-        <v>-0.27310000000000001</v>
+        <v>-0.45150000000000001</v>
       </c>
       <c r="F22">
-        <v>1.1963999999999999</v>
+        <v>0.78784999999999994</v>
       </c>
       <c r="G22">
-        <v>1.4695</v>
+        <v>1.23935</v>
       </c>
       <c r="H22">
         <v>114</v>
@@ -1172,8 +1259,12 @@
       <c r="I22">
         <v>138</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>57</v>
       </c>
@@ -1187,13 +1278,13 @@
         <v>0.22339999999999999</v>
       </c>
       <c r="E23">
-        <v>2.46E-2</v>
+        <v>-0.15379999999999999</v>
       </c>
       <c r="F23">
-        <v>0.22339999999999999</v>
+        <v>-0.18514999999999998</v>
       </c>
       <c r="G23">
-        <v>0.19879999999999998</v>
+        <v>-3.1349999999999989E-2</v>
       </c>
       <c r="H23">
         <v>48</v>
@@ -1201,8 +1292,12 @@
       <c r="I23">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>34</v>
       </c>
@@ -1216,13 +1311,13 @@
         <v>0.53779999999999994</v>
       </c>
       <c r="E24">
-        <v>-2.41E-2</v>
+        <v>-0.20250000000000001</v>
       </c>
       <c r="F24">
-        <v>0.53779999999999994</v>
+        <v>0.12924999999999998</v>
       </c>
       <c r="G24">
-        <v>0.56189999999999996</v>
+        <v>0.33174999999999999</v>
       </c>
       <c r="H24">
         <v>88</v>
@@ -1230,8 +1325,12 @@
       <c r="I24">
         <v>84</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>60</v>
       </c>
@@ -1245,13 +1344,13 @@
         <v>0.33779999999999999</v>
       </c>
       <c r="E25">
-        <v>8.7800000000000003E-2</v>
+        <v>-9.06E-2</v>
       </c>
       <c r="F25">
-        <v>0.33779999999999999</v>
+        <v>-7.074999999999998E-2</v>
       </c>
       <c r="G25">
-        <v>0.25</v>
+        <v>1.985000000000002E-2</v>
       </c>
       <c r="H25">
         <v>59</v>
@@ -1259,8 +1358,12 @@
       <c r="I25">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1288,8 +1391,12 @@
       <c r="I26">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1317,8 +1424,12 @@
       <c r="I27">
         <v>71</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1346,8 +1457,12 @@
       <c r="I28">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>5</v>
       </c>
@@ -1375,8 +1490,12 @@
       <c r="I29">
         <v>59</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -1404,8 +1523,12 @@
       <c r="I30">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>6</v>
       </c>
@@ -1433,8 +1556,12 @@
       <c r="I31">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -1462,8 +1589,12 @@
       <c r="I32">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>8</v>
       </c>
@@ -1491,8 +1622,12 @@
       <c r="I33">
         <v>54</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1520,8 +1655,12 @@
       <c r="I34">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>10</v>
       </c>
@@ -1549,8 +1688,12 @@
       <c r="I35">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -1578,8 +1721,12 @@
       <c r="I36">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>12</v>
       </c>
@@ -1607,8 +1754,12 @@
       <c r="I37">
         <v>71</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>75</v>
       </c>
@@ -1636,8 +1787,12 @@
       <c r="I38">
         <v>51</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>97</v>
       </c>
@@ -1665,8 +1820,12 @@
       <c r="I39">
         <v>149</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>76</v>
       </c>
@@ -1694,8 +1853,12 @@
       <c r="I40">
         <v>66</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>101</v>
       </c>
@@ -1723,8 +1886,12 @@
       <c r="I41">
         <v>81</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J41" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>77</v>
       </c>
@@ -1752,8 +1919,12 @@
       <c r="I42">
         <v>80</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J42" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>102</v>
       </c>
@@ -1781,8 +1952,12 @@
       <c r="I43">
         <v>13</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J43" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>79</v>
       </c>
@@ -1810,8 +1985,12 @@
       <c r="I44">
         <v>57</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J44" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>104</v>
       </c>
@@ -1839,8 +2018,12 @@
       <c r="I45">
         <v>114</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J45" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>81</v>
       </c>
@@ -1868,8 +2051,12 @@
       <c r="I46">
         <v>63</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J46" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>105</v>
       </c>
@@ -1897,8 +2084,12 @@
       <c r="I47">
         <v>155</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J47" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>84</v>
       </c>
@@ -1926,8 +2117,12 @@
       <c r="I48">
         <v>96</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J48" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>108</v>
       </c>
@@ -1955,8 +2150,12 @@
       <c r="I49">
         <v>54</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J49" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>145</v>
       </c>
@@ -1984,8 +2183,12 @@
       <c r="I50">
         <v>56</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J50" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>169</v>
       </c>
@@ -2013,8 +2216,12 @@
       <c r="I51">
         <v>46</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J51" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>147</v>
       </c>
@@ -2042,8 +2249,12 @@
       <c r="I52">
         <v>36</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J52" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>172</v>
       </c>
@@ -2071,8 +2282,12 @@
       <c r="I53">
         <v>39</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J53" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>149</v>
       </c>
@@ -2100,8 +2315,12 @@
       <c r="I54">
         <v>56</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J54" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>174</v>
       </c>
@@ -2129,8 +2348,12 @@
       <c r="I55">
         <v>45</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J55" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>153</v>
       </c>
@@ -2158,8 +2381,12 @@
       <c r="I56">
         <v>71</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J56" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>175</v>
       </c>
@@ -2187,8 +2414,12 @@
       <c r="I57">
         <v>18</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J57" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>154</v>
       </c>
@@ -2216,8 +2447,12 @@
       <c r="I58">
         <v>66</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J58" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>177</v>
       </c>
@@ -2245,8 +2480,12 @@
       <c r="I59">
         <v>45</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J59" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>155</v>
       </c>
@@ -2274,8 +2513,12 @@
       <c r="I60">
         <v>23</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J60" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>180</v>
       </c>
@@ -2303,8 +2546,12 @@
       <c r="I61">
         <v>30</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J61" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>19</v>
       </c>
@@ -2332,8 +2579,12 @@
       <c r="I62">
         <v>62</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J62" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>121</v>
       </c>
@@ -2361,8 +2612,12 @@
       <c r="I63">
         <v>49</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J63" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>20</v>
       </c>
@@ -2390,8 +2645,12 @@
       <c r="I64">
         <v>89</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J64" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>125</v>
       </c>
@@ -2419,8 +2678,12 @@
       <c r="I65">
         <v>7</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J65" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>21</v>
       </c>
@@ -2448,8 +2711,12 @@
       <c r="I66">
         <v>113</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J66" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>126</v>
       </c>
@@ -2477,8 +2744,12 @@
       <c r="I67">
         <v>6</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J67" s="3" t="str">
+        <f t="shared" ref="J67:J130" si="1">IF(E67=C67,"Yes", "No")</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>22</v>
       </c>
@@ -2506,8 +2777,12 @@
       <c r="I68">
         <v>59</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J68" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>127</v>
       </c>
@@ -2535,8 +2810,12 @@
       <c r="I69">
         <v>14</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J69" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>23</v>
       </c>
@@ -2564,8 +2843,12 @@
       <c r="I70">
         <v>5</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J70" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>129</v>
       </c>
@@ -2593,8 +2876,12 @@
       <c r="I71">
         <v>44</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J71" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>24</v>
       </c>
@@ -2622,8 +2909,12 @@
       <c r="I72">
         <v>9</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J72" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>131</v>
       </c>
@@ -2651,8 +2942,12 @@
       <c r="I73">
         <v>23</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J73" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>194</v>
       </c>
@@ -2680,8 +2975,12 @@
       <c r="I74">
         <v>16</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J74" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>218</v>
       </c>
@@ -2709,8 +3008,12 @@
       <c r="I75">
         <v>42</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J75" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>195</v>
       </c>
@@ -2738,8 +3041,12 @@
       <c r="I76">
         <v>32</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J76" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>219</v>
       </c>
@@ -2767,8 +3074,12 @@
       <c r="I77">
         <v>50</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J77" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>198</v>
       </c>
@@ -2796,8 +3107,12 @@
       <c r="I78">
         <v>12</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J78" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>220</v>
       </c>
@@ -2825,8 +3140,12 @@
       <c r="I79">
         <v>6</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J79" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>200</v>
       </c>
@@ -2854,8 +3173,12 @@
       <c r="I80">
         <v>34</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J80" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>223</v>
       </c>
@@ -2883,8 +3206,12 @@
       <c r="I81">
         <v>11</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J81" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>201</v>
       </c>
@@ -2912,8 +3239,12 @@
       <c r="I82">
         <v>43</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J82" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>224</v>
       </c>
@@ -2941,8 +3272,12 @@
       <c r="I83">
         <v>22</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J83" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>204</v>
       </c>
@@ -2970,8 +3305,12 @@
       <c r="I84">
         <v>34</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J84" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>228</v>
       </c>
@@ -2999,8 +3338,12 @@
       <c r="I85">
         <v>6</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J85" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>37</v>
       </c>
@@ -3028,8 +3371,12 @@
       <c r="I86">
         <v>35</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J86" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>61</v>
       </c>
@@ -3057,8 +3404,12 @@
       <c r="I87">
         <v>21</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J87" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>38</v>
       </c>
@@ -3086,8 +3437,12 @@
       <c r="I88">
         <v>35</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J88" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>64</v>
       </c>
@@ -3115,8 +3470,12 @@
       <c r="I89">
         <v>18</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J89" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>41</v>
       </c>
@@ -3144,8 +3503,12 @@
       <c r="I90">
         <v>3</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J90" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>65</v>
       </c>
@@ -3173,8 +3536,12 @@
       <c r="I91">
         <v>15</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J91" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>45</v>
       </c>
@@ -3202,8 +3569,12 @@
       <c r="I92">
         <v>3</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J92" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>68</v>
       </c>
@@ -3231,8 +3602,12 @@
       <c r="I93">
         <v>17</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J93" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>47</v>
       </c>
@@ -3260,8 +3635,12 @@
       <c r="I94">
         <v>20</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J94" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>70</v>
       </c>
@@ -3289,8 +3668,12 @@
       <c r="I95">
         <v>27</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J95" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>48</v>
       </c>
@@ -3318,8 +3701,12 @@
       <c r="I96">
         <v>6</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J96" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>72</v>
       </c>
@@ -3347,8 +3734,12 @@
       <c r="I97">
         <v>26</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J97" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>85</v>
       </c>
@@ -3376,8 +3767,12 @@
       <c r="I98">
         <v>6</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J98" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>109</v>
       </c>
@@ -3405,8 +3800,12 @@
       <c r="I99">
         <v>52</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J99" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>88</v>
       </c>
@@ -3434,8 +3833,12 @@
       <c r="I100">
         <v>8</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J100" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>110</v>
       </c>
@@ -3463,8 +3866,12 @@
       <c r="I101">
         <v>19</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J101" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>90</v>
       </c>
@@ -3492,8 +3899,12 @@
       <c r="I102">
         <v>12</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J102" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>114</v>
       </c>
@@ -3521,8 +3932,12 @@
       <c r="I103">
         <v>7</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J103" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>92</v>
       </c>
@@ -3550,8 +3965,12 @@
       <c r="I104">
         <v>15</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J104" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>118</v>
       </c>
@@ -3579,8 +3998,12 @@
       <c r="I105">
         <v>28</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J105" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>93</v>
       </c>
@@ -3608,8 +4031,12 @@
       <c r="I106">
         <v>2</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J106" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>119</v>
       </c>
@@ -3637,8 +4064,12 @@
       <c r="I107">
         <v>10</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J107" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>95</v>
       </c>
@@ -3666,8 +4097,12 @@
       <c r="I108">
         <v>8</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J108" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>120</v>
       </c>
@@ -3695,8 +4130,12 @@
       <c r="I109">
         <v>40</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J109" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>25</v>
       </c>
@@ -3724,8 +4163,12 @@
       <c r="I110">
         <v>9</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J110" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>134</v>
       </c>
@@ -3753,8 +4196,12 @@
       <c r="I111">
         <v>10</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J111" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>26</v>
       </c>
@@ -3782,8 +4229,12 @@
       <c r="I112">
         <v>53</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J112" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>135</v>
       </c>
@@ -3811,8 +4262,12 @@
       <c r="I113">
         <v>14</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J113" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>27</v>
       </c>
@@ -3840,8 +4295,12 @@
       <c r="I114">
         <v>13</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J114" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>138</v>
       </c>
@@ -3869,8 +4328,12 @@
       <c r="I115">
         <v>19</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J115" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>28</v>
       </c>
@@ -3898,8 +4361,12 @@
       <c r="I116">
         <v>47</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J116" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>139</v>
       </c>
@@ -3927,8 +4394,12 @@
       <c r="I117">
         <v>39</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J117" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>29</v>
       </c>
@@ -3956,8 +4427,12 @@
       <c r="I118">
         <v>21</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J118" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>142</v>
       </c>
@@ -3985,8 +4460,12 @@
       <c r="I119">
         <v>44</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J119" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>30</v>
       </c>
@@ -4014,8 +4493,12 @@
       <c r="I120">
         <v>20</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J120" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>143</v>
       </c>
@@ -4043,8 +4526,12 @@
       <c r="I121">
         <v>21</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J121" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>157</v>
       </c>
@@ -4072,8 +4559,12 @@
       <c r="I122">
         <v>4</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J122" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>181</v>
       </c>
@@ -4101,8 +4592,12 @@
       <c r="I123">
         <v>29</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J123" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>159</v>
       </c>
@@ -4130,8 +4625,12 @@
       <c r="I124">
         <v>7</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J124" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>184</v>
       </c>
@@ -4159,8 +4658,12 @@
       <c r="I125">
         <v>16</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J125" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>162</v>
       </c>
@@ -4188,8 +4691,12 @@
       <c r="I126">
         <v>16</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J126" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>186</v>
       </c>
@@ -4217,8 +4724,12 @@
       <c r="I127">
         <v>51</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J127" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>166</v>
       </c>
@@ -4246,8 +4757,12 @@
       <c r="I128">
         <v>15</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J128" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>187</v>
       </c>
@@ -4275,8 +4790,12 @@
       <c r="I129">
         <v>24</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J129" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>167</v>
       </c>
@@ -4304,8 +4823,12 @@
       <c r="I130">
         <v>23</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J130" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>189</v>
       </c>
@@ -4333,8 +4856,12 @@
       <c r="I131">
         <v>27</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J131" s="3" t="str">
+        <f t="shared" ref="J131:J194" si="2">IF(E131=C131,"Yes", "No")</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>168</v>
       </c>
@@ -4362,8 +4889,12 @@
       <c r="I132" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J132" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>192</v>
       </c>
@@ -4391,8 +4922,12 @@
       <c r="I133">
         <v>61</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J133" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>206</v>
       </c>
@@ -4420,8 +4955,12 @@
       <c r="I134">
         <v>26</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J134" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>229</v>
       </c>
@@ -4449,8 +4988,12 @@
       <c r="I135">
         <v>16</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J135" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>208</v>
       </c>
@@ -4478,8 +5021,12 @@
       <c r="I136">
         <v>11</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J136" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>230</v>
       </c>
@@ -4507,8 +5054,12 @@
       <c r="I137">
         <v>46</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J137" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>207</v>
       </c>
@@ -4536,8 +5087,12 @@
       <c r="I138">
         <v>11</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J138" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>232</v>
       </c>
@@ -4565,8 +5120,12 @@
       <c r="I139">
         <v>2</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J139" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>212</v>
       </c>
@@ -4594,8 +5153,12 @@
       <c r="I140">
         <v>8</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J140" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>235</v>
       </c>
@@ -4623,8 +5186,12 @@
       <c r="I141">
         <v>51</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J141" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>214</v>
       </c>
@@ -4652,8 +5219,12 @@
       <c r="I142">
         <v>35</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J142" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>236</v>
       </c>
@@ -4681,8 +5252,12 @@
       <c r="I143">
         <v>42</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J143" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>216</v>
       </c>
@@ -4710,8 +5285,12 @@
       <c r="I144">
         <v>5</v>
       </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J144" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>237</v>
       </c>
@@ -4739,8 +5318,12 @@
       <c r="I145">
         <v>8</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J145" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>31</v>
       </c>
@@ -4768,8 +5351,12 @@
       <c r="I146">
         <v>34</v>
       </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J146" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>242</v>
       </c>
@@ -4797,8 +5384,12 @@
       <c r="I147">
         <v>0.66700000000000004</v>
       </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J147" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>32</v>
       </c>
@@ -4826,8 +5417,12 @@
       <c r="I148">
         <v>6</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J148" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>244</v>
       </c>
@@ -4855,8 +5450,12 @@
       <c r="I149">
         <v>24</v>
       </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J149" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>33</v>
       </c>
@@ -4884,8 +5483,12 @@
       <c r="I150">
         <v>32</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J150" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>245</v>
       </c>
@@ -4913,8 +5516,12 @@
       <c r="I151">
         <v>13</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J151" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>34</v>
       </c>
@@ -4942,8 +5549,12 @@
       <c r="I152">
         <v>35</v>
       </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J152" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>247</v>
       </c>
@@ -4971,8 +5582,12 @@
       <c r="I153">
         <v>7</v>
       </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J153" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>35</v>
       </c>
@@ -5000,8 +5615,12 @@
       <c r="I154">
         <v>49</v>
       </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J154" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>248</v>
       </c>
@@ -5029,8 +5648,12 @@
       <c r="I155">
         <v>11</v>
       </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J155" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>36</v>
       </c>
@@ -5058,8 +5681,12 @@
       <c r="I156">
         <v>19</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J156" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>250</v>
       </c>
@@ -5087,8 +5714,12 @@
       <c r="I157">
         <v>17</v>
       </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J157" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>265</v>
       </c>
@@ -5116,8 +5747,12 @@
       <c r="I158">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J158" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>291</v>
       </c>
@@ -5145,8 +5780,12 @@
       <c r="I159">
         <v>32</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J159" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>267</v>
       </c>
@@ -5174,28 +5813,32 @@
       <c r="I160">
         <v>47</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J160" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>292</v>
       </c>
       <c r="B161" s="1">
         <v>43851</v>
       </c>
-      <c r="C161">
-        <v>0.41449999999999998</v>
-      </c>
-      <c r="D161">
-        <v>0.58809999999999996</v>
-      </c>
-      <c r="E161">
-        <v>-3.6383333333333323E-2</v>
-      </c>
-      <c r="F161">
-        <v>-3.4058333333333302E-2</v>
-      </c>
-      <c r="G161">
-        <v>2.3250000000000215E-3</v>
+      <c r="C161" t="s">
+        <v>12</v>
+      </c>
+      <c r="D161" t="s">
+        <v>12</v>
+      </c>
+      <c r="E161" t="s">
+        <v>12</v>
+      </c>
+      <c r="F161" t="s">
+        <v>12</v>
+      </c>
+      <c r="G161" t="s">
+        <v>12</v>
       </c>
       <c r="H161" t="s">
         <v>12</v>
@@ -5203,8 +5846,12 @@
       <c r="I161" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J161" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>270</v>
       </c>
@@ -5232,8 +5879,12 @@
       <c r="I162">
         <v>26</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J162" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>294</v>
       </c>
@@ -5261,8 +5912,12 @@
       <c r="I163">
         <v>15</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J163" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>273</v>
       </c>
@@ -5290,8 +5945,12 @@
       <c r="I164">
         <v>58</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J164" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>297</v>
       </c>
@@ -5319,8 +5978,12 @@
       <c r="I165">
         <v>4</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J165" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>274</v>
       </c>
@@ -5348,8 +6011,12 @@
       <c r="I166">
         <v>24</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J166" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>298</v>
       </c>
@@ -5377,8 +6044,12 @@
       <c r="I167">
         <v>6</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J167" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>276</v>
       </c>
@@ -5406,8 +6077,12 @@
       <c r="I168">
         <v>36</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J168" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>299</v>
       </c>
@@ -5435,8 +6110,12 @@
       <c r="I169">
         <v>3</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J169" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>314</v>
       </c>
@@ -5464,8 +6143,12 @@
       <c r="I170">
         <v>8</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J170" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>337</v>
       </c>
@@ -5493,8 +6176,12 @@
       <c r="I171">
         <v>14</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J171" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>316</v>
       </c>
@@ -5522,8 +6209,12 @@
       <c r="I172">
         <v>13</v>
       </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J172" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>338</v>
       </c>
@@ -5551,8 +6242,12 @@
       <c r="I173">
         <v>49</v>
       </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J173" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>318</v>
       </c>
@@ -5580,8 +6275,12 @@
       <c r="I174">
         <v>21</v>
       </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J174" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>341</v>
       </c>
@@ -5609,8 +6308,12 @@
       <c r="I175">
         <v>36</v>
       </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J175" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>319</v>
       </c>
@@ -5638,8 +6341,12 @@
       <c r="I176">
         <v>26</v>
       </c>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J176" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>343</v>
       </c>
@@ -5667,8 +6374,12 @@
       <c r="I177">
         <v>37</v>
       </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J177" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>322</v>
       </c>
@@ -5696,8 +6407,12 @@
       <c r="I178">
         <v>17</v>
       </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J178" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>346</v>
       </c>
@@ -5725,8 +6440,12 @@
       <c r="I179">
         <v>17</v>
       </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J179" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>323</v>
       </c>
@@ -5754,8 +6473,12 @@
       <c r="I180">
         <v>16</v>
       </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J180" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>348</v>
       </c>
@@ -5783,8 +6506,12 @@
       <c r="I181">
         <v>9</v>
       </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J181" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>37</v>
       </c>
@@ -5812,8 +6539,12 @@
       <c r="I182">
         <v>30</v>
       </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J182" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>256</v>
       </c>
@@ -5841,8 +6572,12 @@
       <c r="I183">
         <v>7</v>
       </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J183" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>38</v>
       </c>
@@ -5870,8 +6605,12 @@
       <c r="I184">
         <v>13</v>
       </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J184" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>255</v>
       </c>
@@ -5899,8 +6638,12 @@
       <c r="I185">
         <v>8</v>
       </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J185" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>39</v>
       </c>
@@ -5928,8 +6671,12 @@
       <c r="I186">
         <v>20</v>
       </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J186" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>257</v>
       </c>
@@ -5957,8 +6704,12 @@
       <c r="I187">
         <v>13</v>
       </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J187" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>40</v>
       </c>
@@ -5986,8 +6737,12 @@
       <c r="I188">
         <v>20</v>
       </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J188" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>260</v>
       </c>
@@ -6015,8 +6770,12 @@
       <c r="I189">
         <v>2</v>
       </c>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J189" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>41</v>
       </c>
@@ -6044,8 +6803,12 @@
       <c r="I190">
         <v>9</v>
       </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J190" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>263</v>
       </c>
@@ -6073,8 +6836,12 @@
       <c r="I191">
         <v>21</v>
       </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J191" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>42</v>
       </c>
@@ -6102,8 +6869,12 @@
       <c r="I192">
         <v>8</v>
       </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J192" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>264</v>
       </c>
@@ -6131,8 +6902,12 @@
       <c r="I193">
         <v>2.778</v>
       </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J193" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>279</v>
       </c>
@@ -6160,8 +6935,12 @@
       <c r="I194">
         <v>50</v>
       </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J194" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>308</v>
       </c>
@@ -6189,8 +6968,12 @@
       <c r="I195">
         <v>20</v>
       </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J195" s="3" t="str">
+        <f t="shared" ref="J195:J217" si="3">IF(E195=C195,"Yes", "No")</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>281</v>
       </c>
@@ -6218,8 +7001,12 @@
       <c r="I196">
         <v>55</v>
       </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J196" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>310</v>
       </c>
@@ -6247,8 +7034,12 @@
       <c r="I197">
         <v>36</v>
       </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J197" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>282</v>
       </c>
@@ -6276,8 +7067,12 @@
       <c r="I198">
         <v>33</v>
       </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J198" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>312</v>
       </c>
@@ -6305,8 +7100,12 @@
       <c r="I199">
         <v>59</v>
       </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J199" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>286</v>
       </c>
@@ -6334,8 +7133,12 @@
       <c r="I200">
         <v>2.8889999999999998</v>
       </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J200" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>302</v>
       </c>
@@ -6363,8 +7166,12 @@
       <c r="I201">
         <v>175</v>
       </c>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J201" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>287</v>
       </c>
@@ -6392,8 +7199,12 @@
       <c r="I202">
         <v>53</v>
       </c>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J202" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>304</v>
       </c>
@@ -6421,8 +7232,12 @@
       <c r="I203">
         <v>18</v>
       </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J203" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>288</v>
       </c>
@@ -6450,8 +7265,12 @@
       <c r="I204">
         <v>1.333</v>
       </c>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J204" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>306</v>
       </c>
@@ -6479,8 +7298,12 @@
       <c r="I205">
         <v>36</v>
       </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J205" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>325</v>
       </c>
@@ -6508,8 +7331,12 @@
       <c r="I206">
         <v>22</v>
       </c>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J206" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>351</v>
       </c>
@@ -6537,8 +7364,12 @@
       <c r="I207">
         <v>116</v>
       </c>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J207" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A208">
         <v>327</v>
       </c>
@@ -6566,8 +7397,12 @@
       <c r="I208">
         <v>41</v>
       </c>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J208" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>353</v>
       </c>
@@ -6595,8 +7430,12 @@
       <c r="I209">
         <v>82</v>
       </c>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J209" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>330</v>
       </c>
@@ -6624,8 +7463,12 @@
       <c r="I210">
         <v>11</v>
       </c>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J210" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>354</v>
       </c>
@@ -6653,8 +7496,12 @@
       <c r="I211">
         <v>47</v>
       </c>
-    </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J211" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>333</v>
       </c>
@@ -6682,8 +7529,12 @@
       <c r="I212">
         <v>36</v>
       </c>
-    </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J212" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>355</v>
       </c>
@@ -6711,8 +7562,12 @@
       <c r="I213">
         <v>57</v>
       </c>
-    </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J213" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>334</v>
       </c>
@@ -6740,8 +7595,12 @@
       <c r="I214">
         <v>4.3330000000000002</v>
       </c>
-    </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J214" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>357</v>
       </c>
@@ -6769,8 +7628,12 @@
       <c r="I215">
         <v>44</v>
       </c>
-    </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J215" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>335</v>
       </c>
@@ -6798,8 +7661,12 @@
       <c r="I216">
         <v>79</v>
       </c>
-    </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J216" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>359</v>
       </c>
@@ -6827,8 +7694,13 @@
       <c r="I217">
         <v>26</v>
       </c>
+      <c r="J217" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed values that transferred weird and reran dataframe creation. PnR data cleaned just includes PnR values per billions cells.
</commit_message>
<xml_diff>
--- a/Data/PnR/Jan_Polyp_PnR.xlsx
+++ b/Data/PnR/Jan_Polyp_PnR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jennica Moffat\Documents\CSUNthesis\Data\PnR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C4049E-E701-4A0B-BB7C-84C570822A94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90BBB87-5E4F-4445-9FCC-511498F5F54D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9DE3BF4D-FA46-474F-BFB9-F399C340B799}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$217</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$217</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,9 +37,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
-  <si>
-    <t>PolypID</t>
-  </si>
   <si>
     <t>DarkSlope</t>
   </si>
@@ -175,24 +172,21 @@
   <si>
     <t>Date</t>
   </si>
+  <si>
+    <t>WellNum</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF1E1E1E"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -215,11 +209,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,46 +527,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265D603E-FBC4-405A-8933-8CCF9B7CF3A0}">
-  <dimension ref="A1:J217"/>
+  <dimension ref="A1:I217"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>43851</v>
@@ -599,12 +592,8 @@
       <c r="I2">
         <v>9</v>
       </c>
-      <c r="J2" s="3" t="str">
-        <f>IF(E2=C2,"Yes", "No")</f>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>15</v>
       </c>
@@ -632,14 +621,10 @@
       <c r="I3">
         <v>35</v>
       </c>
-      <c r="J3" s="3" t="str">
-        <f t="shared" ref="J3:J66" si="0">IF(E3=C3,"Yes", "No")</f>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>43851</v>
@@ -665,12 +650,8 @@
       <c r="I4">
         <v>37</v>
       </c>
-      <c r="J4" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>16</v>
       </c>
@@ -698,14 +679,10 @@
       <c r="I5">
         <v>18</v>
       </c>
-      <c r="J5" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>43851</v>
@@ -731,12 +708,8 @@
       <c r="I6">
         <v>48</v>
       </c>
-      <c r="J6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>18</v>
       </c>
@@ -764,14 +737,10 @@
       <c r="I7">
         <v>10</v>
       </c>
-      <c r="J7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>43851</v>
@@ -797,12 +766,8 @@
       <c r="I8">
         <v>21</v>
       </c>
-      <c r="J8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>20</v>
       </c>
@@ -830,45 +795,37 @@
       <c r="I9">
         <v>24</v>
       </c>
-      <c r="J9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>43851</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>22</v>
       </c>
@@ -896,14 +853,10 @@
       <c r="I11">
         <v>38</v>
       </c>
-      <c r="J11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>43851</v>
@@ -929,12 +882,8 @@
       <c r="I12">
         <v>41</v>
       </c>
-      <c r="J12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>24</v>
       </c>
@@ -962,12 +911,8 @@
       <c r="I13">
         <v>11</v>
       </c>
-      <c r="J13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>27</v>
       </c>
@@ -995,12 +940,8 @@
       <c r="I14">
         <v>111</v>
       </c>
-      <c r="J14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>52</v>
       </c>
@@ -1028,12 +969,8 @@
       <c r="I15">
         <v>73</v>
       </c>
-      <c r="J15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>28</v>
       </c>
@@ -1061,12 +998,8 @@
       <c r="I16">
         <v>12</v>
       </c>
-      <c r="J16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>53</v>
       </c>
@@ -1074,32 +1007,28 @@
         <v>43850</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I17" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>29</v>
       </c>
@@ -1127,12 +1056,8 @@
       <c r="I18">
         <v>80</v>
       </c>
-      <c r="J18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>54</v>
       </c>
@@ -1160,12 +1085,8 @@
       <c r="I19">
         <v>110</v>
       </c>
-      <c r="J19" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>32</v>
       </c>
@@ -1193,12 +1114,8 @@
       <c r="I20">
         <v>91</v>
       </c>
-      <c r="J20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>56</v>
       </c>
@@ -1226,12 +1143,8 @@
       <c r="I21">
         <v>54</v>
       </c>
-      <c r="J21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>33</v>
       </c>
@@ -1259,12 +1172,8 @@
       <c r="I22">
         <v>138</v>
       </c>
-      <c r="J22" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>57</v>
       </c>
@@ -1292,12 +1201,8 @@
       <c r="I23">
         <v>56</v>
       </c>
-      <c r="J23" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>34</v>
       </c>
@@ -1325,12 +1230,8 @@
       <c r="I24">
         <v>84</v>
       </c>
-      <c r="J24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>60</v>
       </c>
@@ -1358,14 +1259,10 @@
       <c r="I25">
         <v>58</v>
       </c>
-      <c r="J25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1">
         <v>43850</v>
@@ -1391,12 +1288,8 @@
       <c r="I26">
         <v>27</v>
       </c>
-      <c r="J26" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1424,14 +1317,10 @@
       <c r="I27">
         <v>71</v>
       </c>
-      <c r="J27" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B28" s="1">
         <v>43850</v>
@@ -1457,12 +1346,8 @@
       <c r="I28">
         <v>25</v>
       </c>
-      <c r="J28" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>5</v>
       </c>
@@ -1490,14 +1375,10 @@
       <c r="I29">
         <v>59</v>
       </c>
-      <c r="J29" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30" s="1">
         <v>43850</v>
@@ -1523,12 +1404,8 @@
       <c r="I30">
         <v>40</v>
       </c>
-      <c r="J30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>6</v>
       </c>
@@ -1556,14 +1433,10 @@
       <c r="I31">
         <v>10</v>
       </c>
-      <c r="J31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" s="1">
         <v>43850</v>
@@ -1589,12 +1462,8 @@
       <c r="I32">
         <v>17</v>
       </c>
-      <c r="J32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>8</v>
       </c>
@@ -1622,14 +1491,10 @@
       <c r="I33">
         <v>54</v>
       </c>
-      <c r="J33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="1">
         <v>43850</v>
@@ -1655,12 +1520,8 @@
       <c r="I34">
         <v>23</v>
       </c>
-      <c r="J34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>10</v>
       </c>
@@ -1688,14 +1549,10 @@
       <c r="I35">
         <v>69</v>
       </c>
-      <c r="J35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36" s="1">
         <v>43850</v>
@@ -1721,12 +1578,8 @@
       <c r="I36">
         <v>10</v>
       </c>
-      <c r="J36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>12</v>
       </c>
@@ -1754,12 +1607,8 @@
       <c r="I37">
         <v>71</v>
       </c>
-      <c r="J37" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>75</v>
       </c>
@@ -1787,12 +1636,8 @@
       <c r="I38">
         <v>51</v>
       </c>
-      <c r="J38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>97</v>
       </c>
@@ -1820,12 +1665,8 @@
       <c r="I39">
         <v>149</v>
       </c>
-      <c r="J39" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>76</v>
       </c>
@@ -1853,12 +1694,8 @@
       <c r="I40">
         <v>66</v>
       </c>
-      <c r="J40" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>101</v>
       </c>
@@ -1886,12 +1723,8 @@
       <c r="I41">
         <v>81</v>
       </c>
-      <c r="J41" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>77</v>
       </c>
@@ -1919,12 +1752,8 @@
       <c r="I42">
         <v>80</v>
       </c>
-      <c r="J42" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>102</v>
       </c>
@@ -1952,12 +1781,8 @@
       <c r="I43">
         <v>13</v>
       </c>
-      <c r="J43" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>79</v>
       </c>
@@ -1985,12 +1810,8 @@
       <c r="I44">
         <v>57</v>
       </c>
-      <c r="J44" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>104</v>
       </c>
@@ -2018,12 +1839,8 @@
       <c r="I45">
         <v>114</v>
       </c>
-      <c r="J45" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>81</v>
       </c>
@@ -2051,12 +1868,8 @@
       <c r="I46">
         <v>63</v>
       </c>
-      <c r="J46" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>105</v>
       </c>
@@ -2084,12 +1897,8 @@
       <c r="I47">
         <v>155</v>
       </c>
-      <c r="J47" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>84</v>
       </c>
@@ -2117,12 +1926,8 @@
       <c r="I48">
         <v>96</v>
       </c>
-      <c r="J48" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>108</v>
       </c>
@@ -2150,12 +1955,8 @@
       <c r="I49">
         <v>54</v>
       </c>
-      <c r="J49" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>145</v>
       </c>
@@ -2183,12 +1984,8 @@
       <c r="I50">
         <v>56</v>
       </c>
-      <c r="J50" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>169</v>
       </c>
@@ -2216,12 +2013,8 @@
       <c r="I51">
         <v>46</v>
       </c>
-      <c r="J51" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>147</v>
       </c>
@@ -2249,12 +2042,8 @@
       <c r="I52">
         <v>36</v>
       </c>
-      <c r="J52" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>172</v>
       </c>
@@ -2282,12 +2071,8 @@
       <c r="I53">
         <v>39</v>
       </c>
-      <c r="J53" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>149</v>
       </c>
@@ -2315,12 +2100,8 @@
       <c r="I54">
         <v>56</v>
       </c>
-      <c r="J54" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>174</v>
       </c>
@@ -2348,12 +2129,8 @@
       <c r="I55">
         <v>45</v>
       </c>
-      <c r="J55" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>153</v>
       </c>
@@ -2381,12 +2158,8 @@
       <c r="I56">
         <v>71</v>
       </c>
-      <c r="J56" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>175</v>
       </c>
@@ -2414,12 +2187,8 @@
       <c r="I57">
         <v>18</v>
       </c>
-      <c r="J57" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>154</v>
       </c>
@@ -2447,12 +2216,8 @@
       <c r="I58">
         <v>66</v>
       </c>
-      <c r="J58" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>177</v>
       </c>
@@ -2480,12 +2245,8 @@
       <c r="I59">
         <v>45</v>
       </c>
-      <c r="J59" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>155</v>
       </c>
@@ -2513,12 +2274,8 @@
       <c r="I60">
         <v>23</v>
       </c>
-      <c r="J60" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>180</v>
       </c>
@@ -2546,14 +2303,10 @@
       <c r="I61">
         <v>30</v>
       </c>
-      <c r="J61" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B62" s="1">
         <v>43850</v>
@@ -2579,12 +2332,8 @@
       <c r="I62">
         <v>62</v>
       </c>
-      <c r="J62" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>121</v>
       </c>
@@ -2612,14 +2361,10 @@
       <c r="I63">
         <v>49</v>
       </c>
-      <c r="J63" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B64" s="1">
         <v>43850</v>
@@ -2645,12 +2390,8 @@
       <c r="I64">
         <v>89</v>
       </c>
-      <c r="J64" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>125</v>
       </c>
@@ -2678,14 +2419,10 @@
       <c r="I65">
         <v>7</v>
       </c>
-      <c r="J65" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B66" s="1">
         <v>43850</v>
@@ -2711,12 +2448,8 @@
       <c r="I66">
         <v>113</v>
       </c>
-      <c r="J66" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>126</v>
       </c>
@@ -2744,14 +2477,10 @@
       <c r="I67">
         <v>6</v>
       </c>
-      <c r="J67" s="3" t="str">
-        <f t="shared" ref="J67:J130" si="1">IF(E67=C67,"Yes", "No")</f>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B68" s="1">
         <v>43850</v>
@@ -2777,12 +2506,8 @@
       <c r="I68">
         <v>59</v>
       </c>
-      <c r="J68" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>127</v>
       </c>
@@ -2810,14 +2535,10 @@
       <c r="I69">
         <v>14</v>
       </c>
-      <c r="J69" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B70" s="1">
         <v>43850</v>
@@ -2843,12 +2564,8 @@
       <c r="I70">
         <v>5</v>
       </c>
-      <c r="J70" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>129</v>
       </c>
@@ -2876,14 +2593,10 @@
       <c r="I71">
         <v>44</v>
       </c>
-      <c r="J71" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B72" s="1">
         <v>43850</v>
@@ -2909,12 +2622,8 @@
       <c r="I72">
         <v>9</v>
       </c>
-      <c r="J72" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>131</v>
       </c>
@@ -2942,12 +2651,8 @@
       <c r="I73">
         <v>23</v>
       </c>
-      <c r="J73" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>194</v>
       </c>
@@ -2975,12 +2680,8 @@
       <c r="I74">
         <v>16</v>
       </c>
-      <c r="J74" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>218</v>
       </c>
@@ -3008,12 +2709,8 @@
       <c r="I75">
         <v>42</v>
       </c>
-      <c r="J75" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>195</v>
       </c>
@@ -3041,12 +2738,8 @@
       <c r="I76">
         <v>32</v>
       </c>
-      <c r="J76" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>219</v>
       </c>
@@ -3074,12 +2767,8 @@
       <c r="I77">
         <v>50</v>
       </c>
-      <c r="J77" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>198</v>
       </c>
@@ -3107,12 +2796,8 @@
       <c r="I78">
         <v>12</v>
       </c>
-      <c r="J78" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>220</v>
       </c>
@@ -3140,12 +2825,8 @@
       <c r="I79">
         <v>6</v>
       </c>
-      <c r="J79" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>200</v>
       </c>
@@ -3173,12 +2854,8 @@
       <c r="I80">
         <v>34</v>
       </c>
-      <c r="J80" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>223</v>
       </c>
@@ -3206,12 +2883,8 @@
       <c r="I81">
         <v>11</v>
       </c>
-      <c r="J81" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>201</v>
       </c>
@@ -3239,12 +2912,8 @@
       <c r="I82">
         <v>43</v>
       </c>
-      <c r="J82" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>224</v>
       </c>
@@ -3272,12 +2941,8 @@
       <c r="I83">
         <v>22</v>
       </c>
-      <c r="J83" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>204</v>
       </c>
@@ -3305,12 +2970,8 @@
       <c r="I84">
         <v>34</v>
       </c>
-      <c r="J84" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>228</v>
       </c>
@@ -3338,12 +2999,8 @@
       <c r="I85">
         <v>6</v>
       </c>
-      <c r="J85" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>37</v>
       </c>
@@ -3371,12 +3028,8 @@
       <c r="I86">
         <v>35</v>
       </c>
-      <c r="J86" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>61</v>
       </c>
@@ -3404,12 +3057,8 @@
       <c r="I87">
         <v>21</v>
       </c>
-      <c r="J87" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>38</v>
       </c>
@@ -3437,12 +3086,8 @@
       <c r="I88">
         <v>35</v>
       </c>
-      <c r="J88" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>64</v>
       </c>
@@ -3470,12 +3115,8 @@
       <c r="I89">
         <v>18</v>
       </c>
-      <c r="J89" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>41</v>
       </c>
@@ -3503,12 +3144,8 @@
       <c r="I90">
         <v>3</v>
       </c>
-      <c r="J90" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>65</v>
       </c>
@@ -3536,12 +3173,8 @@
       <c r="I91">
         <v>15</v>
       </c>
-      <c r="J91" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>45</v>
       </c>
@@ -3569,12 +3202,8 @@
       <c r="I92">
         <v>3</v>
       </c>
-      <c r="J92" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>68</v>
       </c>
@@ -3602,12 +3231,8 @@
       <c r="I93">
         <v>17</v>
       </c>
-      <c r="J93" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>47</v>
       </c>
@@ -3635,12 +3260,8 @@
       <c r="I94">
         <v>20</v>
       </c>
-      <c r="J94" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>70</v>
       </c>
@@ -3668,12 +3289,8 @@
       <c r="I95">
         <v>27</v>
       </c>
-      <c r="J95" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>48</v>
       </c>
@@ -3701,12 +3318,8 @@
       <c r="I96">
         <v>6</v>
       </c>
-      <c r="J96" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>72</v>
       </c>
@@ -3734,12 +3347,8 @@
       <c r="I97">
         <v>26</v>
       </c>
-      <c r="J97" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>85</v>
       </c>
@@ -3767,12 +3376,8 @@
       <c r="I98">
         <v>6</v>
       </c>
-      <c r="J98" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>109</v>
       </c>
@@ -3800,12 +3405,8 @@
       <c r="I99">
         <v>52</v>
       </c>
-      <c r="J99" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>88</v>
       </c>
@@ -3833,12 +3434,8 @@
       <c r="I100">
         <v>8</v>
       </c>
-      <c r="J100" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>110</v>
       </c>
@@ -3866,12 +3463,8 @@
       <c r="I101">
         <v>19</v>
       </c>
-      <c r="J101" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>90</v>
       </c>
@@ -3899,12 +3492,8 @@
       <c r="I102">
         <v>12</v>
       </c>
-      <c r="J102" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>114</v>
       </c>
@@ -3932,12 +3521,8 @@
       <c r="I103">
         <v>7</v>
       </c>
-      <c r="J103" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>92</v>
       </c>
@@ -3965,12 +3550,8 @@
       <c r="I104">
         <v>15</v>
       </c>
-      <c r="J104" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>118</v>
       </c>
@@ -3998,12 +3579,8 @@
       <c r="I105">
         <v>28</v>
       </c>
-      <c r="J105" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>93</v>
       </c>
@@ -4031,12 +3608,8 @@
       <c r="I106">
         <v>2</v>
       </c>
-      <c r="J106" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>119</v>
       </c>
@@ -4064,12 +3637,8 @@
       <c r="I107">
         <v>10</v>
       </c>
-      <c r="J107" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>95</v>
       </c>
@@ -4097,12 +3666,8 @@
       <c r="I108">
         <v>8</v>
       </c>
-      <c r="J108" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>120</v>
       </c>
@@ -4130,14 +3695,10 @@
       <c r="I109">
         <v>40</v>
       </c>
-      <c r="J109" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B110" s="1">
         <v>43851</v>
@@ -4163,12 +3724,8 @@
       <c r="I110">
         <v>9</v>
       </c>
-      <c r="J110" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>134</v>
       </c>
@@ -4196,14 +3753,10 @@
       <c r="I111">
         <v>10</v>
       </c>
-      <c r="J111" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B112" s="1">
         <v>43851</v>
@@ -4229,12 +3782,8 @@
       <c r="I112">
         <v>53</v>
       </c>
-      <c r="J112" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>135</v>
       </c>
@@ -4262,14 +3811,10 @@
       <c r="I113">
         <v>14</v>
       </c>
-      <c r="J113" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B114" s="1">
         <v>43851</v>
@@ -4295,12 +3840,8 @@
       <c r="I114">
         <v>13</v>
       </c>
-      <c r="J114" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>138</v>
       </c>
@@ -4328,14 +3869,10 @@
       <c r="I115">
         <v>19</v>
       </c>
-      <c r="J115" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B116" s="1">
         <v>43851</v>
@@ -4361,12 +3898,8 @@
       <c r="I116">
         <v>47</v>
       </c>
-      <c r="J116" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>139</v>
       </c>
@@ -4394,14 +3927,10 @@
       <c r="I117">
         <v>39</v>
       </c>
-      <c r="J117" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B118" s="1">
         <v>43851</v>
@@ -4427,12 +3956,8 @@
       <c r="I118">
         <v>21</v>
       </c>
-      <c r="J118" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>142</v>
       </c>
@@ -4460,14 +3985,10 @@
       <c r="I119">
         <v>44</v>
       </c>
-      <c r="J119" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B120" s="1">
         <v>43851</v>
@@ -4493,12 +4014,8 @@
       <c r="I120">
         <v>20</v>
       </c>
-      <c r="J120" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>143</v>
       </c>
@@ -4526,12 +4043,8 @@
       <c r="I121">
         <v>21</v>
       </c>
-      <c r="J121" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>157</v>
       </c>
@@ -4559,12 +4072,8 @@
       <c r="I122">
         <v>4</v>
       </c>
-      <c r="J122" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>181</v>
       </c>
@@ -4592,12 +4101,8 @@
       <c r="I123">
         <v>29</v>
       </c>
-      <c r="J123" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>159</v>
       </c>
@@ -4625,12 +4130,8 @@
       <c r="I124">
         <v>7</v>
       </c>
-      <c r="J124" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>184</v>
       </c>
@@ -4658,12 +4159,8 @@
       <c r="I125">
         <v>16</v>
       </c>
-      <c r="J125" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>162</v>
       </c>
@@ -4691,12 +4188,8 @@
       <c r="I126">
         <v>16</v>
       </c>
-      <c r="J126" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>186</v>
       </c>
@@ -4724,12 +4217,8 @@
       <c r="I127">
         <v>51</v>
       </c>
-      <c r="J127" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>166</v>
       </c>
@@ -4757,12 +4246,8 @@
       <c r="I128">
         <v>15</v>
       </c>
-      <c r="J128" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>187</v>
       </c>
@@ -4790,12 +4275,8 @@
       <c r="I129">
         <v>24</v>
       </c>
-      <c r="J129" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>167</v>
       </c>
@@ -4823,12 +4304,8 @@
       <c r="I130">
         <v>23</v>
       </c>
-      <c r="J130" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>189</v>
       </c>
@@ -4856,12 +4333,8 @@
       <c r="I131">
         <v>27</v>
       </c>
-      <c r="J131" s="3" t="str">
-        <f t="shared" ref="J131:J194" si="2">IF(E131=C131,"Yes", "No")</f>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>168</v>
       </c>
@@ -4884,17 +4357,13 @@
         <v>-3.7549999999999972E-2</v>
       </c>
       <c r="H132" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I132" t="s">
-        <v>12</v>
-      </c>
-      <c r="J132" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>192</v>
       </c>
@@ -4922,12 +4391,8 @@
       <c r="I133">
         <v>61</v>
       </c>
-      <c r="J133" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>206</v>
       </c>
@@ -4955,12 +4420,8 @@
       <c r="I134">
         <v>26</v>
       </c>
-      <c r="J134" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>229</v>
       </c>
@@ -4988,12 +4449,8 @@
       <c r="I135">
         <v>16</v>
       </c>
-      <c r="J135" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>208</v>
       </c>
@@ -5021,12 +4478,8 @@
       <c r="I136">
         <v>11</v>
       </c>
-      <c r="J136" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>230</v>
       </c>
@@ -5054,12 +4507,8 @@
       <c r="I137">
         <v>46</v>
       </c>
-      <c r="J137" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>207</v>
       </c>
@@ -5087,12 +4536,8 @@
       <c r="I138">
         <v>11</v>
       </c>
-      <c r="J138" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>232</v>
       </c>
@@ -5120,12 +4565,8 @@
       <c r="I139">
         <v>2</v>
       </c>
-      <c r="J139" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>212</v>
       </c>
@@ -5153,12 +4594,8 @@
       <c r="I140">
         <v>8</v>
       </c>
-      <c r="J140" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>235</v>
       </c>
@@ -5186,12 +4623,8 @@
       <c r="I141">
         <v>51</v>
       </c>
-      <c r="J141" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>214</v>
       </c>
@@ -5219,12 +4652,8 @@
       <c r="I142">
         <v>35</v>
       </c>
-      <c r="J142" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>236</v>
       </c>
@@ -5252,12 +4681,8 @@
       <c r="I143">
         <v>42</v>
       </c>
-      <c r="J143" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>216</v>
       </c>
@@ -5285,12 +4710,8 @@
       <c r="I144">
         <v>5</v>
       </c>
-      <c r="J144" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>237</v>
       </c>
@@ -5318,14 +4739,10 @@
       <c r="I145">
         <v>8</v>
       </c>
-      <c r="J145" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B146" s="1">
         <v>43851</v>
@@ -5351,12 +4768,8 @@
       <c r="I146">
         <v>34</v>
       </c>
-      <c r="J146" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>242</v>
       </c>
@@ -5384,14 +4797,10 @@
       <c r="I147">
         <v>0.66700000000000004</v>
       </c>
-      <c r="J147" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B148" s="1">
         <v>43851</v>
@@ -5417,12 +4826,8 @@
       <c r="I148">
         <v>6</v>
       </c>
-      <c r="J148" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>244</v>
       </c>
@@ -5450,14 +4855,10 @@
       <c r="I149">
         <v>24</v>
       </c>
-      <c r="J149" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B150" s="1">
         <v>43851</v>
@@ -5483,12 +4884,8 @@
       <c r="I150">
         <v>32</v>
       </c>
-      <c r="J150" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>245</v>
       </c>
@@ -5516,14 +4913,10 @@
       <c r="I151">
         <v>13</v>
       </c>
-      <c r="J151" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B152" s="1">
         <v>43851</v>
@@ -5549,12 +4942,8 @@
       <c r="I152">
         <v>35</v>
       </c>
-      <c r="J152" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>247</v>
       </c>
@@ -5582,14 +4971,10 @@
       <c r="I153">
         <v>7</v>
       </c>
-      <c r="J153" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B154" s="1">
         <v>43851</v>
@@ -5615,12 +5000,8 @@
       <c r="I154">
         <v>49</v>
       </c>
-      <c r="J154" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>248</v>
       </c>
@@ -5648,14 +5029,10 @@
       <c r="I155">
         <v>11</v>
       </c>
-      <c r="J155" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B156" s="1">
         <v>43851</v>
@@ -5681,12 +5058,8 @@
       <c r="I156">
         <v>19</v>
       </c>
-      <c r="J156" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>250</v>
       </c>
@@ -5714,12 +5087,8 @@
       <c r="I157">
         <v>17</v>
       </c>
-      <c r="J157" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>265</v>
       </c>
@@ -5747,12 +5116,8 @@
       <c r="I158">
         <v>0.22</v>
       </c>
-      <c r="J158" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>291</v>
       </c>
@@ -5780,12 +5145,8 @@
       <c r="I159">
         <v>32</v>
       </c>
-      <c r="J159" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>267</v>
       </c>
@@ -5813,12 +5174,8 @@
       <c r="I160">
         <v>47</v>
       </c>
-      <c r="J160" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>292</v>
       </c>
@@ -5826,32 +5183,28 @@
         <v>43851</v>
       </c>
       <c r="C161" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D161" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E161" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F161" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G161" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H161" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I161" t="s">
-        <v>12</v>
-      </c>
-      <c r="J161" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>270</v>
       </c>
@@ -5879,12 +5232,8 @@
       <c r="I162">
         <v>26</v>
       </c>
-      <c r="J162" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>294</v>
       </c>
@@ -5912,12 +5261,8 @@
       <c r="I163">
         <v>15</v>
       </c>
-      <c r="J163" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>273</v>
       </c>
@@ -5945,12 +5290,8 @@
       <c r="I164">
         <v>58</v>
       </c>
-      <c r="J164" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>297</v>
       </c>
@@ -5978,12 +5319,8 @@
       <c r="I165">
         <v>4</v>
       </c>
-      <c r="J165" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>274</v>
       </c>
@@ -6011,12 +5348,8 @@
       <c r="I166">
         <v>24</v>
       </c>
-      <c r="J166" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>298</v>
       </c>
@@ -6044,12 +5377,8 @@
       <c r="I167">
         <v>6</v>
       </c>
-      <c r="J167" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>276</v>
       </c>
@@ -6077,12 +5406,8 @@
       <c r="I168">
         <v>36</v>
       </c>
-      <c r="J168" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>299</v>
       </c>
@@ -6110,12 +5435,8 @@
       <c r="I169">
         <v>3</v>
       </c>
-      <c r="J169" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>314</v>
       </c>
@@ -6143,12 +5464,8 @@
       <c r="I170">
         <v>8</v>
       </c>
-      <c r="J170" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>337</v>
       </c>
@@ -6176,12 +5493,8 @@
       <c r="I171">
         <v>14</v>
       </c>
-      <c r="J171" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>316</v>
       </c>
@@ -6209,12 +5522,8 @@
       <c r="I172">
         <v>13</v>
       </c>
-      <c r="J172" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>338</v>
       </c>
@@ -6242,12 +5551,8 @@
       <c r="I173">
         <v>49</v>
       </c>
-      <c r="J173" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>318</v>
       </c>
@@ -6275,12 +5580,8 @@
       <c r="I174">
         <v>21</v>
       </c>
-      <c r="J174" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>341</v>
       </c>
@@ -6308,12 +5609,8 @@
       <c r="I175">
         <v>36</v>
       </c>
-      <c r="J175" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>319</v>
       </c>
@@ -6341,12 +5638,8 @@
       <c r="I176">
         <v>26</v>
       </c>
-      <c r="J176" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>343</v>
       </c>
@@ -6374,12 +5667,8 @@
       <c r="I177">
         <v>37</v>
       </c>
-      <c r="J177" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>322</v>
       </c>
@@ -6407,12 +5696,8 @@
       <c r="I178">
         <v>17</v>
       </c>
-      <c r="J178" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>346</v>
       </c>
@@ -6440,12 +5725,8 @@
       <c r="I179">
         <v>17</v>
       </c>
-      <c r="J179" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>323</v>
       </c>
@@ -6473,12 +5754,8 @@
       <c r="I180">
         <v>16</v>
       </c>
-      <c r="J180" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>348</v>
       </c>
@@ -6506,14 +5783,10 @@
       <c r="I181">
         <v>9</v>
       </c>
-      <c r="J181" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B182" s="2">
         <v>43852</v>
@@ -6539,12 +5812,8 @@
       <c r="I182">
         <v>30</v>
       </c>
-      <c r="J182" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>256</v>
       </c>
@@ -6572,14 +5841,10 @@
       <c r="I183">
         <v>7</v>
       </c>
-      <c r="J183" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B184" s="2">
         <v>43852</v>
@@ -6605,12 +5870,8 @@
       <c r="I184">
         <v>13</v>
       </c>
-      <c r="J184" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>255</v>
       </c>
@@ -6638,14 +5899,10 @@
       <c r="I185">
         <v>8</v>
       </c>
-      <c r="J185" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B186" s="2">
         <v>43852</v>
@@ -6671,12 +5928,8 @@
       <c r="I186">
         <v>20</v>
       </c>
-      <c r="J186" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>257</v>
       </c>
@@ -6704,14 +5957,10 @@
       <c r="I187">
         <v>13</v>
       </c>
-      <c r="J187" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B188" s="2">
         <v>43852</v>
@@ -6737,12 +5986,8 @@
       <c r="I188">
         <v>20</v>
       </c>
-      <c r="J188" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>260</v>
       </c>
@@ -6770,14 +6015,10 @@
       <c r="I189">
         <v>2</v>
       </c>
-      <c r="J189" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B190" s="2">
         <v>43852</v>
@@ -6803,12 +6044,8 @@
       <c r="I190">
         <v>9</v>
       </c>
-      <c r="J190" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>263</v>
       </c>
@@ -6836,14 +6073,10 @@
       <c r="I191">
         <v>21</v>
       </c>
-      <c r="J191" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B192" s="2">
         <v>43852</v>
@@ -6869,12 +6102,8 @@
       <c r="I192">
         <v>8</v>
       </c>
-      <c r="J192" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>264</v>
       </c>
@@ -6902,12 +6131,8 @@
       <c r="I193">
         <v>2.778</v>
       </c>
-      <c r="J193" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>279</v>
       </c>
@@ -6935,12 +6160,8 @@
       <c r="I194">
         <v>50</v>
       </c>
-      <c r="J194" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>308</v>
       </c>
@@ -6968,12 +6189,8 @@
       <c r="I195">
         <v>20</v>
       </c>
-      <c r="J195" s="3" t="str">
-        <f t="shared" ref="J195:J217" si="3">IF(E195=C195,"Yes", "No")</f>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>281</v>
       </c>
@@ -7001,12 +6218,8 @@
       <c r="I196">
         <v>55</v>
       </c>
-      <c r="J196" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>310</v>
       </c>
@@ -7034,12 +6247,8 @@
       <c r="I197">
         <v>36</v>
       </c>
-      <c r="J197" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>282</v>
       </c>
@@ -7067,12 +6276,8 @@
       <c r="I198">
         <v>33</v>
       </c>
-      <c r="J198" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>312</v>
       </c>
@@ -7100,12 +6305,8 @@
       <c r="I199">
         <v>59</v>
       </c>
-      <c r="J199" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>286</v>
       </c>
@@ -7133,12 +6334,8 @@
       <c r="I200">
         <v>2.8889999999999998</v>
       </c>
-      <c r="J200" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>302</v>
       </c>
@@ -7166,12 +6363,8 @@
       <c r="I201">
         <v>175</v>
       </c>
-      <c r="J201" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>287</v>
       </c>
@@ -7199,12 +6392,8 @@
       <c r="I202">
         <v>53</v>
       </c>
-      <c r="J202" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>304</v>
       </c>
@@ -7232,12 +6421,8 @@
       <c r="I203">
         <v>18</v>
       </c>
-      <c r="J203" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>288</v>
       </c>
@@ -7265,12 +6450,8 @@
       <c r="I204">
         <v>1.333</v>
       </c>
-      <c r="J204" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>306</v>
       </c>
@@ -7298,12 +6479,8 @@
       <c r="I205">
         <v>36</v>
       </c>
-      <c r="J205" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>325</v>
       </c>
@@ -7331,12 +6508,8 @@
       <c r="I206">
         <v>22</v>
       </c>
-      <c r="J206" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>351</v>
       </c>
@@ -7364,12 +6537,8 @@
       <c r="I207">
         <v>116</v>
       </c>
-      <c r="J207" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A208">
         <v>327</v>
       </c>
@@ -7397,12 +6566,8 @@
       <c r="I208">
         <v>41</v>
       </c>
-      <c r="J208" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>353</v>
       </c>
@@ -7430,12 +6595,8 @@
       <c r="I209">
         <v>82</v>
       </c>
-      <c r="J209" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>330</v>
       </c>
@@ -7463,12 +6624,8 @@
       <c r="I210">
         <v>11</v>
       </c>
-      <c r="J210" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>354</v>
       </c>
@@ -7496,12 +6653,8 @@
       <c r="I211">
         <v>47</v>
       </c>
-      <c r="J211" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>333</v>
       </c>
@@ -7529,12 +6682,8 @@
       <c r="I212">
         <v>36</v>
       </c>
-      <c r="J212" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>355</v>
       </c>
@@ -7562,12 +6711,8 @@
       <c r="I213">
         <v>57</v>
       </c>
-      <c r="J213" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>334</v>
       </c>
@@ -7595,12 +6740,8 @@
       <c r="I214">
         <v>4.3330000000000002</v>
       </c>
-      <c r="J214" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>357</v>
       </c>
@@ -7628,12 +6769,8 @@
       <c r="I215">
         <v>44</v>
       </c>
-      <c r="J215" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>335</v>
       </c>
@@ -7661,12 +6798,8 @@
       <c r="I216">
         <v>79</v>
       </c>
-      <c r="J216" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>359</v>
       </c>
@@ -7693,10 +6826,6 @@
       </c>
       <c r="I217">
         <v>26</v>
-      </c>
-      <c r="J217" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>No</v>
       </c>
     </row>
   </sheetData>

</xml_diff>